<commit_message>
Sensors in Dnipro + Leaflet Hash
</commit_message>
<xml_diff>
--- a/doc/Workbook1.xlsx
+++ b/doc/Workbook1.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="224">
   <si>
     <t>senzorvzduchu.cz</t>
   </si>
@@ -322,13 +322,382 @@
   </si>
   <si>
     <t>,"info":"</t>
+  </si>
+  <si>
+    <t>35.049889</t>
+  </si>
+  <si>
+    <t>48.466098</t>
+  </si>
+  <si>
+    <t>DNK1</t>
+  </si>
+  <si>
+    <t>Dnipro</t>
+  </si>
+  <si>
+    <t>savednipro.org</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>35.0460373</t>
+  </si>
+  <si>
+    <t>48.4642516</t>
+  </si>
+  <si>
+    <t>DNK2</t>
+  </si>
+  <si>
+    <t>Heroiv Maidanu Square, bus station, pedestrian area, huge traffic</t>
+  </si>
+  <si>
+    <t>35.0653546</t>
+  </si>
+  <si>
+    <t>48.4663951</t>
+  </si>
+  <si>
+    <t>DNK3</t>
+  </si>
+  <si>
+    <t>Festival pier, pedestrian area, crowded place, the longest promenade in Ukraine</t>
+  </si>
+  <si>
+    <t>35.0733477</t>
+  </si>
+  <si>
+    <t>48.4084019</t>
+  </si>
+  <si>
+    <t>DNK4</t>
+  </si>
+  <si>
+    <t>35.0629357</t>
+  </si>
+  <si>
+    <t>48.4243839</t>
+  </si>
+  <si>
+    <t>DNK5</t>
+  </si>
+  <si>
+    <t>Kosmichnaya Street, roundabout, reference measurement station, huge traffic</t>
+  </si>
+  <si>
+    <t>35.1318213</t>
+  </si>
+  <si>
+    <t>48.4039489</t>
+  </si>
+  <si>
+    <t>DNK6</t>
+  </si>
+  <si>
+    <t>34.9474725</t>
+  </si>
+  <si>
+    <t>48.4872575</t>
+  </si>
+  <si>
+    <t>DNK7</t>
+  </si>
+  <si>
+    <t>Novokodatskyi Park, ice arena, no traffic, city hospital</t>
+  </si>
+  <si>
+    <t>34.9778414</t>
+  </si>
+  <si>
+    <t>48.4761675</t>
+  </si>
+  <si>
+    <t>DNK8</t>
+  </si>
+  <si>
+    <t>Serhiia Nihoiana Avenue, reference measurement station, governmental building, metallurgical plant</t>
+  </si>
+  <si>
+    <t>34.9899219</t>
+  </si>
+  <si>
+    <t>48.509473</t>
+  </si>
+  <si>
+    <t>DNK9</t>
+  </si>
+  <si>
+    <t>35.0141552</t>
+  </si>
+  <si>
+    <t>48.5310254</t>
+  </si>
+  <si>
+    <t>DNK10</t>
+  </si>
+  <si>
+    <t>35.089979</t>
+  </si>
+  <si>
+    <t>48.498245</t>
+  </si>
+  <si>
+    <t>DNK11</t>
+  </si>
+  <si>
+    <t>35.05493</t>
+  </si>
+  <si>
+    <t>48.515423</t>
+  </si>
+  <si>
+    <t>DNK12</t>
+  </si>
+  <si>
+    <t>35.0063704</t>
+  </si>
+  <si>
+    <t>48.4374452</t>
+  </si>
+  <si>
+    <t>DNK13</t>
+  </si>
+  <si>
+    <t>35.0327317</t>
+  </si>
+  <si>
+    <t>48.5266199</t>
+  </si>
+  <si>
+    <t>DNK14</t>
+  </si>
+  <si>
+    <t>35.0152727</t>
+  </si>
+  <si>
+    <t>48.4772814</t>
+  </si>
+  <si>
+    <t>DNK15</t>
+  </si>
+  <si>
+    <t>Central railway station, crowded place, huge traffic</t>
+  </si>
+  <si>
+    <t>35.0228672</t>
+  </si>
+  <si>
+    <t>48.4719534</t>
+  </si>
+  <si>
+    <t>DNK16</t>
+  </si>
+  <si>
+    <t>34.9524035</t>
+  </si>
+  <si>
+    <t>48.5216731</t>
+  </si>
+  <si>
+    <t>DNK17</t>
+  </si>
+  <si>
+    <t>City Cardiac-Hospital #20, Amur-Nyzhnodniprovskyi District, no traffic</t>
+  </si>
+  <si>
+    <t>35.0276852</t>
+  </si>
+  <si>
+    <t>48.3958008</t>
+  </si>
+  <si>
+    <t>DNK18</t>
+  </si>
+  <si>
+    <t>34.9801057</t>
+  </si>
+  <si>
+    <t>48.3936032</t>
+  </si>
+  <si>
+    <t>DNK19</t>
+  </si>
+  <si>
+    <t>35.0010162</t>
+  </si>
+  <si>
+    <t>48.4081437</t>
+  </si>
+  <si>
+    <t>DNK20</t>
+  </si>
+  <si>
+    <t>34.9060767</t>
+  </si>
+  <si>
+    <t>48.480765</t>
+  </si>
+  <si>
+    <t>DNK21</t>
+  </si>
+  <si>
+    <t>35.0231467</t>
+  </si>
+  <si>
+    <t>48.425396</t>
+  </si>
+  <si>
+    <t>DNK22</t>
+  </si>
+  <si>
+    <t>35.0094192</t>
+  </si>
+  <si>
+    <t>48.428169</t>
+  </si>
+  <si>
+    <t>DNK23</t>
+  </si>
+  <si>
+    <t>35.0593666</t>
+  </si>
+  <si>
+    <t>48.450057</t>
+  </si>
+  <si>
+    <t>DNK24</t>
+  </si>
+  <si>
+    <t>34.969635</t>
+  </si>
+  <si>
+    <t>48.461718</t>
+  </si>
+  <si>
+    <t>DNK25</t>
+  </si>
+  <si>
+    <t>35.0009117</t>
+  </si>
+  <si>
+    <t>48.4475965</t>
+  </si>
+  <si>
+    <t>DNK26</t>
+  </si>
+  <si>
+    <t>Kaverina street, shopping malls, farmer's market, schools, huge traffic</t>
+  </si>
+  <si>
+    <t>35.0640127</t>
+  </si>
+  <si>
+    <t>48.4819102</t>
+  </si>
+  <si>
+    <t>DNK27</t>
+  </si>
+  <si>
+    <t>35.0488214</t>
+  </si>
+  <si>
+    <t>48.4916231</t>
+  </si>
+  <si>
+    <t>DNK28</t>
+  </si>
+  <si>
+    <t>Clinical Hospital #9, moderate traffic, schools</t>
+  </si>
+  <si>
+    <t>35.0815529</t>
+  </si>
+  <si>
+    <t>48.4607313</t>
+  </si>
+  <si>
+    <t>DNK29</t>
+  </si>
+  <si>
+    <t>Monastyrskyi island, Aquarium, green area, city park, no traffic</t>
+  </si>
+  <si>
+    <t>35.0700553</t>
+  </si>
+  <si>
+    <t>48.4626939</t>
+  </si>
+  <si>
+    <t>DNK30</t>
+  </si>
+  <si>
+    <t>Shopping mall \"MOST-City\", bus station, entrance to the \"Central bridge\", crowded place</t>
+  </si>
+  <si>
+    <t>Cafe \"Fantaziya\", pedestrian area, small green area, housing area, schools</t>
+  </si>
+  <si>
+    <t>House of culture \"Energetyk\", reference measurement station, residential area</t>
+  </si>
+  <si>
+    <t>Housing area \"Frunzenskyi\", huge traffic, residential area, shopping market</t>
+  </si>
+  <si>
+    <t>Housing area \"Livoberezhnyi-3\", residential area, schools, small traffic</t>
+  </si>
+  <si>
+    <t>Metallurgical plant \"Interpipe\", reference measurement station</t>
+  </si>
+  <si>
+    <t>Market \"Obraztsova\", Kalynova Street, schools, playgrounds, moderate traffic</t>
+  </si>
+  <si>
+    <t>Modern park \"Green Grove\", crowded place, green area, no traffic</t>
+  </si>
+  <si>
+    <t>Shopping mall \"Karavan\", huge traffic, crowded place, large market</t>
+  </si>
+  <si>
+    <t>Central city market \"Ozerka\", large parking slot, huge traffic, crowded place, central park</t>
+  </si>
+  <si>
+    <t>Housing area \"Topolia\", city hospital, schools</t>
+  </si>
+  <si>
+    <t>Housing area \"Krotova\", far from city center, schools, kindergarten</t>
+  </si>
+  <si>
+    <t>Housing area \"Kvartal 12\", large intersection, market, shopping mall, huge traffic, pedestrian area, schools, kindergartens</t>
+  </si>
+  <si>
+    <t>Housing area \"Parus\", schools, pedestrian area, bus station, small traffic</t>
+  </si>
+  <si>
+    <t>Shopping mall \"Dafi\", large roundabout, huge traffic, crowded place</t>
+  </si>
+  <si>
+    <t>Tytova street, shopping mall \"Silpo\", small traffic, residential area, street market, schools, kindergarten</t>
+  </si>
+  <si>
+    <t>Shopping mall \"Nagorka\", huge traffic, universities, hospitals</t>
+  </si>
+  <si>
+    <t>Petrovskogo street, shopping mall \"Varus\", children's clinical hospital #6, groceries stores, huge traffic</t>
+  </si>
+  <si>
+    <t>Housing area \"Solnechnyi\", huge traffic, small city park</t>
+  </si>
+  <si>
+    <t>Park \"Shevchenko\", no traffic, green area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -373,6 +742,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -420,7 +793,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -435,6 +808,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -772,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q21"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22:E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2012,9 +2391,1418 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.3721686,50.0702677]},"properties":{"id":"PRG20","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Main exit to Pilsen, hill, valley."}},</v>
       </c>
     </row>
+    <row r="22" spans="1:19" ht="110" thickBot="1">
+      <c r="A22" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="6">
+        <v>3</v>
+      </c>
+      <c r="G22" s="6">
+        <v>1</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J22" t="s">
+        <v>92</v>
+      </c>
+      <c r="K22" t="s">
+        <v>93</v>
+      </c>
+      <c r="L22" t="s">
+        <v>94</v>
+      </c>
+      <c r="M22" t="s">
+        <v>95</v>
+      </c>
+      <c r="N22" t="s">
+        <v>96</v>
+      </c>
+      <c r="O22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="86" thickBot="1">
+      <c r="A23" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="6">
+        <v>3</v>
+      </c>
+      <c r="G23" s="6">
+        <v>1</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J23" t="s">
+        <v>92</v>
+      </c>
+      <c r="K23" t="s">
+        <v>93</v>
+      </c>
+      <c r="L23" t="s">
+        <v>94</v>
+      </c>
+      <c r="M23" t="s">
+        <v>95</v>
+      </c>
+      <c r="N23" t="s">
+        <v>96</v>
+      </c>
+      <c r="O23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="98" thickBot="1">
+      <c r="A24" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="6">
+        <v>3</v>
+      </c>
+      <c r="G24" s="6">
+        <v>1</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J24" t="s">
+        <v>92</v>
+      </c>
+      <c r="K24" t="s">
+        <v>93</v>
+      </c>
+      <c r="L24" t="s">
+        <v>94</v>
+      </c>
+      <c r="M24" t="s">
+        <v>95</v>
+      </c>
+      <c r="N24" t="s">
+        <v>96</v>
+      </c>
+      <c r="O24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="98" thickBot="1">
+      <c r="A25" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" s="6">
+        <v>3</v>
+      </c>
+      <c r="G25" s="6">
+        <v>0</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J25" t="s">
+        <v>92</v>
+      </c>
+      <c r="K25" t="s">
+        <v>93</v>
+      </c>
+      <c r="L25" t="s">
+        <v>94</v>
+      </c>
+      <c r="M25" t="s">
+        <v>95</v>
+      </c>
+      <c r="N25" t="s">
+        <v>96</v>
+      </c>
+      <c r="O25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="86" thickBot="1">
+      <c r="A26" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="6">
+        <v>3</v>
+      </c>
+      <c r="G26" s="6">
+        <v>1</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J26" t="s">
+        <v>92</v>
+      </c>
+      <c r="K26" t="s">
+        <v>93</v>
+      </c>
+      <c r="L26" t="s">
+        <v>94</v>
+      </c>
+      <c r="M26" t="s">
+        <v>95</v>
+      </c>
+      <c r="N26" t="s">
+        <v>96</v>
+      </c>
+      <c r="O26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="98" thickBot="1">
+      <c r="A27" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="6">
+        <v>3</v>
+      </c>
+      <c r="G27" s="6">
+        <v>0</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J27" t="s">
+        <v>92</v>
+      </c>
+      <c r="K27" t="s">
+        <v>93</v>
+      </c>
+      <c r="L27" t="s">
+        <v>94</v>
+      </c>
+      <c r="M27" t="s">
+        <v>95</v>
+      </c>
+      <c r="N27" t="s">
+        <v>96</v>
+      </c>
+      <c r="O27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="62" thickBot="1">
+      <c r="A28" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" s="6">
+        <v>3</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J28" t="s">
+        <v>92</v>
+      </c>
+      <c r="K28" t="s">
+        <v>93</v>
+      </c>
+      <c r="L28" t="s">
+        <v>94</v>
+      </c>
+      <c r="M28" t="s">
+        <v>95</v>
+      </c>
+      <c r="N28" t="s">
+        <v>96</v>
+      </c>
+      <c r="O28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="122" thickBot="1">
+      <c r="A29" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" s="6">
+        <v>3</v>
+      </c>
+      <c r="G29" s="6">
+        <v>1</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J29" t="s">
+        <v>92</v>
+      </c>
+      <c r="K29" t="s">
+        <v>93</v>
+      </c>
+      <c r="L29" t="s">
+        <v>94</v>
+      </c>
+      <c r="M29" t="s">
+        <v>95</v>
+      </c>
+      <c r="N29" t="s">
+        <v>96</v>
+      </c>
+      <c r="O29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="110" thickBot="1">
+      <c r="A30" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="6">
+        <v>3</v>
+      </c>
+      <c r="G30" s="6">
+        <v>1</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J30" t="s">
+        <v>92</v>
+      </c>
+      <c r="K30" t="s">
+        <v>93</v>
+      </c>
+      <c r="L30" t="s">
+        <v>94</v>
+      </c>
+      <c r="M30" t="s">
+        <v>95</v>
+      </c>
+      <c r="N30" t="s">
+        <v>96</v>
+      </c>
+      <c r="O30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="98" thickBot="1">
+      <c r="A31" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="6">
+        <v>3</v>
+      </c>
+      <c r="G31" s="6">
+        <v>0</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J31" t="s">
+        <v>92</v>
+      </c>
+      <c r="K31" t="s">
+        <v>93</v>
+      </c>
+      <c r="L31" t="s">
+        <v>94</v>
+      </c>
+      <c r="M31" t="s">
+        <v>95</v>
+      </c>
+      <c r="N31" t="s">
+        <v>96</v>
+      </c>
+      <c r="O31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="74" thickBot="1">
+      <c r="A32" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" s="6">
+        <v>3</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J32" t="s">
+        <v>92</v>
+      </c>
+      <c r="K32" t="s">
+        <v>93</v>
+      </c>
+      <c r="L32" t="s">
+        <v>94</v>
+      </c>
+      <c r="M32" t="s">
+        <v>95</v>
+      </c>
+      <c r="N32" t="s">
+        <v>96</v>
+      </c>
+      <c r="O32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="98" thickBot="1">
+      <c r="A33" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F33" s="6">
+        <v>3</v>
+      </c>
+      <c r="G33" s="6">
+        <v>1</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J33" t="s">
+        <v>92</v>
+      </c>
+      <c r="K33" t="s">
+        <v>93</v>
+      </c>
+      <c r="L33" t="s">
+        <v>94</v>
+      </c>
+      <c r="M33" t="s">
+        <v>95</v>
+      </c>
+      <c r="N33" t="s">
+        <v>96</v>
+      </c>
+      <c r="O33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="86" thickBot="1">
+      <c r="A34" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" s="6">
+        <v>3</v>
+      </c>
+      <c r="G34" s="6">
+        <v>0</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J34" t="s">
+        <v>92</v>
+      </c>
+      <c r="K34" t="s">
+        <v>93</v>
+      </c>
+      <c r="L34" t="s">
+        <v>94</v>
+      </c>
+      <c r="M34" t="s">
+        <v>95</v>
+      </c>
+      <c r="N34" t="s">
+        <v>96</v>
+      </c>
+      <c r="O34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="86" thickBot="1">
+      <c r="A35" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F35" s="6">
+        <v>3</v>
+      </c>
+      <c r="G35" s="6">
+        <v>1</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J35" t="s">
+        <v>92</v>
+      </c>
+      <c r="K35" t="s">
+        <v>93</v>
+      </c>
+      <c r="L35" t="s">
+        <v>94</v>
+      </c>
+      <c r="M35" t="s">
+        <v>95</v>
+      </c>
+      <c r="N35" t="s">
+        <v>96</v>
+      </c>
+      <c r="O35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="74" thickBot="1">
+      <c r="A36" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F36" s="6">
+        <v>3</v>
+      </c>
+      <c r="G36" s="6">
+        <v>1</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J36" t="s">
+        <v>92</v>
+      </c>
+      <c r="K36" t="s">
+        <v>93</v>
+      </c>
+      <c r="L36" t="s">
+        <v>94</v>
+      </c>
+      <c r="M36" t="s">
+        <v>95</v>
+      </c>
+      <c r="N36" t="s">
+        <v>96</v>
+      </c>
+      <c r="O36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="110" thickBot="1">
+      <c r="A37" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37" s="6">
+        <v>3</v>
+      </c>
+      <c r="G37" s="6">
+        <v>1</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J37" t="s">
+        <v>92</v>
+      </c>
+      <c r="K37" t="s">
+        <v>93</v>
+      </c>
+      <c r="L37" t="s">
+        <v>94</v>
+      </c>
+      <c r="M37" t="s">
+        <v>95</v>
+      </c>
+      <c r="N37" t="s">
+        <v>96</v>
+      </c>
+      <c r="O37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="86" thickBot="1">
+      <c r="A38" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F38" s="6">
+        <v>3</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J38" t="s">
+        <v>92</v>
+      </c>
+      <c r="K38" t="s">
+        <v>93</v>
+      </c>
+      <c r="L38" t="s">
+        <v>94</v>
+      </c>
+      <c r="M38" t="s">
+        <v>95</v>
+      </c>
+      <c r="N38" t="s">
+        <v>96</v>
+      </c>
+      <c r="O38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="62" thickBot="1">
+      <c r="A39" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F39" s="6">
+        <v>3</v>
+      </c>
+      <c r="G39" s="6">
+        <v>1</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J39" t="s">
+        <v>92</v>
+      </c>
+      <c r="K39" t="s">
+        <v>93</v>
+      </c>
+      <c r="L39" t="s">
+        <v>94</v>
+      </c>
+      <c r="M39" t="s">
+        <v>95</v>
+      </c>
+      <c r="N39" t="s">
+        <v>96</v>
+      </c>
+      <c r="O39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="86" thickBot="1">
+      <c r="A40" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F40" s="6">
+        <v>3</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J40" t="s">
+        <v>92</v>
+      </c>
+      <c r="K40" t="s">
+        <v>93</v>
+      </c>
+      <c r="L40" t="s">
+        <v>94</v>
+      </c>
+      <c r="M40" t="s">
+        <v>95</v>
+      </c>
+      <c r="N40" t="s">
+        <v>96</v>
+      </c>
+      <c r="O40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="170" thickBot="1">
+      <c r="A41" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F41" s="6">
+        <v>3</v>
+      </c>
+      <c r="G41" s="6">
+        <v>1</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J41" t="s">
+        <v>92</v>
+      </c>
+      <c r="K41" t="s">
+        <v>93</v>
+      </c>
+      <c r="L41" t="s">
+        <v>94</v>
+      </c>
+      <c r="M41" t="s">
+        <v>95</v>
+      </c>
+      <c r="N41" t="s">
+        <v>96</v>
+      </c>
+      <c r="O41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="98" thickBot="1">
+      <c r="A42" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F42" s="6">
+        <v>3</v>
+      </c>
+      <c r="G42" s="6">
+        <v>0</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J42" t="s">
+        <v>92</v>
+      </c>
+      <c r="K42" t="s">
+        <v>93</v>
+      </c>
+      <c r="L42" t="s">
+        <v>94</v>
+      </c>
+      <c r="M42" t="s">
+        <v>95</v>
+      </c>
+      <c r="N42" t="s">
+        <v>96</v>
+      </c>
+      <c r="O42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="86" thickBot="1">
+      <c r="A43" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F43" s="6">
+        <v>3</v>
+      </c>
+      <c r="G43" s="6">
+        <v>1</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J43" t="s">
+        <v>92</v>
+      </c>
+      <c r="K43" t="s">
+        <v>93</v>
+      </c>
+      <c r="L43" t="s">
+        <v>94</v>
+      </c>
+      <c r="M43" t="s">
+        <v>95</v>
+      </c>
+      <c r="N43" t="s">
+        <v>96</v>
+      </c>
+      <c r="O43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="134" thickBot="1">
+      <c r="A44" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F44" s="6">
+        <v>3</v>
+      </c>
+      <c r="G44" s="6">
+        <v>0</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J44" t="s">
+        <v>92</v>
+      </c>
+      <c r="K44" t="s">
+        <v>93</v>
+      </c>
+      <c r="L44" t="s">
+        <v>94</v>
+      </c>
+      <c r="M44" t="s">
+        <v>95</v>
+      </c>
+      <c r="N44" t="s">
+        <v>96</v>
+      </c>
+      <c r="O44" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="74" thickBot="1">
+      <c r="A45" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F45" s="6">
+        <v>3</v>
+      </c>
+      <c r="G45" s="6">
+        <v>1</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J45" t="s">
+        <v>92</v>
+      </c>
+      <c r="K45" t="s">
+        <v>93</v>
+      </c>
+      <c r="L45" t="s">
+        <v>94</v>
+      </c>
+      <c r="M45" t="s">
+        <v>95</v>
+      </c>
+      <c r="N45" t="s">
+        <v>96</v>
+      </c>
+      <c r="O45" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="134" thickBot="1">
+      <c r="A46" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F46" s="6">
+        <v>3</v>
+      </c>
+      <c r="G46" s="6">
+        <v>1</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J46" t="s">
+        <v>92</v>
+      </c>
+      <c r="K46" t="s">
+        <v>93</v>
+      </c>
+      <c r="L46" t="s">
+        <v>94</v>
+      </c>
+      <c r="M46" t="s">
+        <v>95</v>
+      </c>
+      <c r="N46" t="s">
+        <v>96</v>
+      </c>
+      <c r="O46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="98" thickBot="1">
+      <c r="A47" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F47" s="6">
+        <v>3</v>
+      </c>
+      <c r="G47" s="6">
+        <v>1</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J47" t="s">
+        <v>92</v>
+      </c>
+      <c r="K47" t="s">
+        <v>93</v>
+      </c>
+      <c r="L47" t="s">
+        <v>94</v>
+      </c>
+      <c r="M47" t="s">
+        <v>95</v>
+      </c>
+      <c r="N47" t="s">
+        <v>96</v>
+      </c>
+      <c r="O47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="74" thickBot="1">
+      <c r="A48" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F48" s="6">
+        <v>3</v>
+      </c>
+      <c r="G48" s="6">
+        <v>1</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J48" t="s">
+        <v>92</v>
+      </c>
+      <c r="K48" t="s">
+        <v>93</v>
+      </c>
+      <c r="L48" t="s">
+        <v>94</v>
+      </c>
+      <c r="M48" t="s">
+        <v>95</v>
+      </c>
+      <c r="N48" t="s">
+        <v>96</v>
+      </c>
+      <c r="O48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="62" thickBot="1">
+      <c r="A49" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F49" s="6">
+        <v>3</v>
+      </c>
+      <c r="G49" s="6">
+        <v>0</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J49" t="s">
+        <v>92</v>
+      </c>
+      <c r="K49" t="s">
+        <v>93</v>
+      </c>
+      <c r="L49" t="s">
+        <v>94</v>
+      </c>
+      <c r="M49" t="s">
+        <v>95</v>
+      </c>
+      <c r="N49" t="s">
+        <v>96</v>
+      </c>
+      <c r="O49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="74" thickBot="1">
+      <c r="A50" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F50" s="6">
+        <v>3</v>
+      </c>
+      <c r="G50" s="6">
+        <v>0</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J50" t="s">
+        <v>92</v>
+      </c>
+      <c r="K50" t="s">
+        <v>93</v>
+      </c>
+      <c r="L50" t="s">
+        <v>94</v>
+      </c>
+      <c r="M50" t="s">
+        <v>95</v>
+      </c>
+      <c r="N50" t="s">
+        <v>96</v>
+      </c>
+      <c r="O50" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="62" thickBot="1">
+      <c r="A51" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F51" s="6">
+        <v>3</v>
+      </c>
+      <c r="G51" s="6">
+        <v>0</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J51" t="s">
+        <v>92</v>
+      </c>
+      <c r="K51" t="s">
+        <v>93</v>
+      </c>
+      <c r="L51" t="s">
+        <v>94</v>
+      </c>
+      <c r="M51" t="s">
+        <v>95</v>
+      </c>
+      <c r="N51" t="s">
+        <v>96</v>
+      </c>
+      <c r="O51" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
update Prague add Rennes
</commit_message>
<xml_diff>
--- a/doc/Workbook1.xlsx
+++ b/doc/Workbook1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1894" uniqueCount="450">
   <si>
     <t>senzorvzduchu.cz</t>
   </si>
@@ -1475,7 +1475,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1488,6 +1488,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1543,7 +1544,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1557,6 +1558,7 @@
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1894,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H90" workbookViewId="0">
-      <selection activeCell="S98" sqref="S98:S118"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1903,7 +1905,7 @@
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16" thickBot="1">
+    <row r="1" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1932,7 +1934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="86" thickBot="1">
+    <row r="2" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1992,7 +1994,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.4301362,50.0756786]},"properties":{"id":"PRG1","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Busy intersection with people, traffic, schools and hospital nearby."}},</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="182" thickBot="1">
+    <row r="3" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -2052,7 +2054,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.4306759,50.0723734]},"properties":{"id":"PRG2","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Traffic sensor, but also a refence point to CHMIs http://portal.chmi.cz/files/portal/docs/uoco/web_generator/locality/pollution_locality/loc_ALEG_CZ.html"}},</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="38" thickBot="1">
+    <row r="4" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -2112,7 +2114,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.434207,50.0737929]},"properties":{"id":"PRG3","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":0,"info":"Residential area with school."}},</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="182" thickBot="1">
+    <row r="5" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -2172,7 +2174,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.4427897,50.081394]},"properties":{"id":"PRG4","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":0,"info":"Reference measurement to CHMI AIM station in park Riegrovy sady: http://portal.chmi.cz/files/portal/docs/uoco/web_generator/locality/pollution_locality/loc_ARIE_CZ.html"}},</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="62" thickBot="1">
+    <row r="6" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
@@ -2232,7 +2234,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.4379673,50.0910011]},"properties":{"id":"PRG5","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Busy intersection, under overpass, bus station."}},</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="98" thickBot="1">
+    <row r="7" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
@@ -2292,7 +2294,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.414311,50.0860711]},"properties":{"id":"PRG6","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Transit through UNESCO World Heritage site 21000 cars/working day."}},</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="62" thickBot="1">
+    <row r="8" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -2352,7 +2354,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.4085724,50.0724672]},"properties":{"id":"PRG7","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Busy intersection with people and traffic, riverside."}},</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="38" thickBot="1">
+    <row r="9" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
@@ -2412,7 +2414,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.4050826,50.0749651]},"properties":{"id":"PRG8","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Busy road with people and traffic."}},</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="206" thickBot="1">
+    <row r="10" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -2472,7 +2474,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.3993835,50.0716768]},"properties":{"id":"PRG9","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Traffic from Pilsen x Blanka tunnel. Above the tunnel is also a CHMI AIM http://portal.chmi.cz/files/portal/docs/uoco/web_generator/locality/pollution_locality/loc_ASMI_CZ.html"}},</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="50" thickBot="1">
+    <row r="11" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
@@ -2532,7 +2534,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.3821469,50.0893636]},"properties":{"id":"PRG10","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Residential area, exits from Blanka tunnel."}},</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="74" thickBot="1">
+    <row r="12" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A12" s="2" t="s">
         <v>52</v>
       </c>
@@ -2592,7 +2594,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.3964891,50.1002118]},"properties":{"id":"PRG11","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Farmers market, huge roundabout, heavy traffic to airport."}},</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="50" thickBot="1">
+    <row r="13" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A13" s="2" t="s">
         <v>56</v>
       </c>
@@ -2652,7 +2654,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.4442736,50.1147822]},"properties":{"id":"PRG12","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Exit from tunnel Blanka, riverside."}},</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="62" thickBot="1">
+    <row r="14" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
@@ -2712,7 +2714,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.4611478,50.1176375]},"properties":{"id":"PRG13","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Residential area on hill with 90.000 cars/working day."}},</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="50" thickBot="1">
+    <row r="15" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
@@ -2772,7 +2774,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.4434085,50.1032446]},"properties":{"id":"PRG14","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Busy road, Vltava river level, Billa parking."}},</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="50" thickBot="1">
+    <row r="16" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A16" s="2" t="s">
         <v>68</v>
       </c>
@@ -2832,7 +2834,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.4810011,50.1043091]},"properties":{"id":"PRG15","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Busy intersection, gas station, overpass."}},</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="62" thickBot="1">
+    <row r="17" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A17" s="2" t="s">
         <v>72</v>
       </c>
@@ -2892,7 +2894,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.4665657,50.0691655]},"properties":{"id":"PRG16","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Road in walley, parking, Ministry of enviroment."}},</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="122" thickBot="1">
+    <row r="18" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A18" s="2" t="s">
         <v>76</v>
       </c>
@@ -2952,7 +2954,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.4807536,50.0486962]},"properties":{"id":"PRG17","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"120.000 cars/working day with a lot of heavy trucks due to lack of the south - east - north transit ring around Prague."}},</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="26" thickBot="1">
+    <row r="19" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A19" s="2" t="s">
         <v>80</v>
       </c>
@@ -3012,7 +3014,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.4101525,50.0336998]},"properties":{"id":"PRG18","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Busy bridge intersection."}},</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="38" thickBot="1">
+    <row r="20" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A20" s="2" t="s">
         <v>84</v>
       </c>
@@ -3072,7 +3074,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.4094995,50.0609116]},"properties":{"id":"PRG19","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Bus station, heavy traffic nearby."}},</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="38" thickBot="1">
+    <row r="21" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A21" s="2" t="s">
         <v>88</v>
       </c>
@@ -3132,7 +3134,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[14.3721686,50.0702677]},"properties":{"id":"PRG20","group":"senzorvzduchu.cz","city":"Prague","color":"#00cc99","height":3,"trafic":1,"info":"Main exit to Pilsen, hill, valley."}},</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="110" thickBot="1">
+    <row r="22" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A22" s="6" t="s">
         <v>101</v>
       </c>
@@ -3192,7 +3194,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.049889,48.466098]},"properties":{"id":"DNK1","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Shopping mall \"MOST-City\", bus station, entrance to the \"Central bridge\", crowded place"}},</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="86" thickBot="1">
+    <row r="23" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A23" s="6" t="s">
         <v>107</v>
       </c>
@@ -3252,7 +3254,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0460373,48.4642516]},"properties":{"id":"DNK2","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Heroiv Maidanu Square, bus station, pedestrian area, huge traffic"}},</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="98" thickBot="1">
+    <row r="24" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A24" s="6" t="s">
         <v>111</v>
       </c>
@@ -3312,7 +3314,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0653546,48.4663951]},"properties":{"id":"DNK3","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Festival pier, pedestrian area, crowded place, the longest promenade in Ukraine"}},</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="98" thickBot="1">
+    <row r="25" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A25" s="6" t="s">
         <v>115</v>
       </c>
@@ -3372,7 +3374,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0733477,48.4084019]},"properties":{"id":"DNK4","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":0,"info":"Cafe \"Fantaziya\", pedestrian area, small green area, housing area, schools"}},</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="86" thickBot="1">
+    <row r="26" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A26" s="6" t="s">
         <v>118</v>
       </c>
@@ -3432,7 +3434,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0629357,48.4243839]},"properties":{"id":"DNK5","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Kosmichnaya Street, roundabout, reference measurement station, huge traffic"}},</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="98" thickBot="1">
+    <row r="27" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A27" s="6" t="s">
         <v>122</v>
       </c>
@@ -3492,7 +3494,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.1318213,48.4039489]},"properties":{"id":"DNK6","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":0,"info":"House of culture \"Energetyk\", reference measurement station, residential area"}},</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="62" thickBot="1">
+    <row r="28" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A28" s="6" t="s">
         <v>125</v>
       </c>
@@ -3552,7 +3554,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[34.9474725,48.4872575]},"properties":{"id":"DNK7","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":0,"info":"Novokodatskyi Park, ice arena, no traffic, city hospital"}},</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="122" thickBot="1">
+    <row r="29" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A29" s="6" t="s">
         <v>129</v>
       </c>
@@ -3612,7 +3614,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[34.9778414,48.4761675]},"properties":{"id":"DNK8","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Serhiia Nihoiana Avenue, reference measurement station, governmental building, metallurgical plant"}},</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="110" thickBot="1">
+    <row r="30" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A30" s="6" t="s">
         <v>133</v>
       </c>
@@ -3672,7 +3674,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[34.9899219,48.509473]},"properties":{"id":"DNK9","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Housing area \"Frunzenskyi\", huge traffic, residential area, shopping market"}},</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="98" thickBot="1">
+    <row r="31" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A31" s="6" t="s">
         <v>136</v>
       </c>
@@ -3732,7 +3734,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0141552,48.5310254]},"properties":{"id":"DNK10","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":0,"info":"Housing area \"Livoberezhnyi-3\", residential area, schools, small traffic"}},</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="74" thickBot="1">
+    <row r="32" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A32" s="6" t="s">
         <v>139</v>
       </c>
@@ -3792,7 +3794,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.089979,48.498245]},"properties":{"id":"DNK11","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":0,"info":"Metallurgical plant \"Interpipe\", reference measurement station"}},</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="98" thickBot="1">
+    <row r="33" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A33" s="6" t="s">
         <v>142</v>
       </c>
@@ -3852,7 +3854,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.05493,48.515423]},"properties":{"id":"DNK12","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Market \"Obraztsova\", Kalynova Street, schools, playgrounds, moderate traffic"}},</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="86" thickBot="1">
+    <row r="34" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A34" s="6" t="s">
         <v>145</v>
       </c>
@@ -3912,7 +3914,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0063704,48.4374452]},"properties":{"id":"DNK13","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":0,"info":"Modern park \"Green Grove\", crowded place, green area, no traffic"}},</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="86" thickBot="1">
+    <row r="35" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A35" s="6" t="s">
         <v>148</v>
       </c>
@@ -3972,7 +3974,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0327317,48.5266199]},"properties":{"id":"DNK14","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Shopping mall \"Karavan\", huge traffic, crowded place, large market"}},</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="74" thickBot="1">
+    <row r="36" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A36" s="6" t="s">
         <v>151</v>
       </c>
@@ -4032,7 +4034,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0152727,48.4772814]},"properties":{"id":"DNK15","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Central railway station, crowded place, huge traffic"}},</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="110" thickBot="1">
+    <row r="37" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A37" s="6" t="s">
         <v>155</v>
       </c>
@@ -4092,7 +4094,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0228672,48.4719534]},"properties":{"id":"DNK16","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Central city market \"Ozerka\", large parking slot, huge traffic, crowded place, central park"}},</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="86" thickBot="1">
+    <row r="38" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A38" s="6" t="s">
         <v>158</v>
       </c>
@@ -4152,7 +4154,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[34.9524035,48.5216731]},"properties":{"id":"DNK17","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":0,"info":"City Cardiac-Hospital #20, Amur-Nyzhnodniprovskyi District, no traffic"}},</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="62" thickBot="1">
+    <row r="39" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A39" s="6" t="s">
         <v>162</v>
       </c>
@@ -4212,7 +4214,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0276852,48.3958008]},"properties":{"id":"DNK18","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Housing area \"Topolia\", city hospital, schools"}},</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="86" thickBot="1">
+    <row r="40" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A40" s="6" t="s">
         <v>165</v>
       </c>
@@ -4272,7 +4274,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[34.9801057,48.3936032]},"properties":{"id":"DNK19","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":0,"info":"Housing area \"Krotova\", far from city center, schools, kindergarten"}},</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="170" thickBot="1">
+    <row r="41" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A41" s="6" t="s">
         <v>168</v>
       </c>
@@ -4332,7 +4334,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0010162,48.4081437]},"properties":{"id":"DNK20","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Housing area \"Kvartal 12\", large intersection, market, shopping mall, huge traffic, pedestrian area, schools, kindergartens"}},</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="98" thickBot="1">
+    <row r="42" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A42" s="6" t="s">
         <v>171</v>
       </c>
@@ -4392,7 +4394,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[34.9060767,48.480765]},"properties":{"id":"DNK21","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":0,"info":"Housing area \"Parus\", schools, pedestrian area, bus station, small traffic"}},</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="86" thickBot="1">
+    <row r="43" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A43" s="6" t="s">
         <v>174</v>
       </c>
@@ -4452,7 +4454,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0231467,48.425396]},"properties":{"id":"DNK22","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Shopping mall \"Dafi\", large roundabout, huge traffic, crowded place"}},</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="134" thickBot="1">
+    <row r="44" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A44" s="6" t="s">
         <v>177</v>
       </c>
@@ -4512,7 +4514,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0094192,48.428169]},"properties":{"id":"DNK23","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":0,"info":"Tytova street, shopping mall \"Silpo\", small traffic, residential area, street market, schools, kindergarten"}},</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="74" thickBot="1">
+    <row r="45" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A45" s="6" t="s">
         <v>180</v>
       </c>
@@ -4572,7 +4574,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0593666,48.450057]},"properties":{"id":"DNK24","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Shopping mall \"Nagorka\", huge traffic, universities, hospitals"}},</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="134" thickBot="1">
+    <row r="46" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A46" s="6" t="s">
         <v>183</v>
       </c>
@@ -4632,7 +4634,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[34.969635,48.461718]},"properties":{"id":"DNK25","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Petrovskogo street, shopping mall \"Varus\", children's clinical hospital #6, groceries stores, huge traffic"}},</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="98" thickBot="1">
+    <row r="47" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A47" s="6" t="s">
         <v>186</v>
       </c>
@@ -4692,7 +4694,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0009117,48.4475965]},"properties":{"id":"DNK26","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Kaverina street, shopping malls, farmer's market, schools, huge traffic"}},</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="74" thickBot="1">
+    <row r="48" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A48" s="6" t="s">
         <v>190</v>
       </c>
@@ -4752,7 +4754,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0640127,48.4819102]},"properties":{"id":"DNK27","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":1,"info":"Housing area \"Solnechnyi\", huge traffic, small city park"}},</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="62" thickBot="1">
+    <row r="49" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A49" s="6" t="s">
         <v>193</v>
       </c>
@@ -4812,7 +4814,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0488214,48.4916231]},"properties":{"id":"DNK28","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":0,"info":"Clinical Hospital #9, moderate traffic, schools"}},</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="74" thickBot="1">
+    <row r="50" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A50" s="6" t="s">
         <v>197</v>
       </c>
@@ -4872,7 +4874,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0815529,48.4607313]},"properties":{"id":"DNK29","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":0,"info":"Monastyrskyi island, Aquarium, green area, city park, no traffic"}},</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="62" thickBot="1">
+    <row r="51" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A51" s="6" t="s">
         <v>201</v>
       </c>
@@ -4932,7 +4934,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[35.0700553,48.4626939]},"properties":{"id":"DNK30","group":"savednipro.org","city":"Dnipro","color":"#000000","height":3,"trafic":0,"info":"Park \"Shevchenko\", no traffic, green area"}},</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="97">
+    <row r="52" spans="1:19" ht="28" customHeight="1">
       <c r="A52" s="8" t="s">
         <v>224</v>
       </c>
@@ -4992,7 +4994,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.075728,47.467912]},"properties":{"id":"BUD1","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Közvágóhíd megálló) Busy intersection with people. traffic. party places. theatre nearby."}},</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="145">
+    <row r="53" spans="1:19" ht="28" customHeight="1">
       <c r="A53" s="8" t="s">
         <v>231</v>
       </c>
@@ -5052,7 +5054,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.080888,47.466466]},"properties":{"id":"BUD2","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Near Közvágóhíd. Gubacsi út Tesco) moderate busy road close to intersection. people. traffic. party places. and mall close."}},</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="97">
+    <row r="54" spans="1:19" ht="28" customHeight="1">
       <c r="A54" s="8" t="s">
         <v>235</v>
       </c>
@@ -5062,7 +5064,9 @@
       <c r="C54" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="D54" s="8"/>
+      <c r="D54" s="8" t="s">
+        <v>227</v>
+      </c>
       <c r="E54" s="8" t="s">
         <v>228</v>
       </c>
@@ -5107,10 +5111,10 @@
       </c>
       <c r="S54" t="str">
         <f t="shared" si="0"/>
-        <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.067378,47.479634]},"properties":{"id":"BUD3","group":"CAAG","city":"","color":"#3fc9f0","height":2,"trafic":1,"info":"(Boráros tér-fent) Busy intersection. bus station. with people. traffic. many office buildings."}},</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" ht="85">
+        <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.067378,47.479634]},"properties":{"id":"BUD3","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Boráros tér-fent) Busy intersection. bus station. with people. traffic. many office buildings."}},</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" ht="28" customHeight="1">
       <c r="A55" s="8" t="s">
         <v>239</v>
       </c>
@@ -5170,7 +5174,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.066933,47.479971]},"properties":{"id":"BUD4","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1,"trafic":1,"info":"(Boráros tér -lent) Busy intersection with people. traffic. many office buildings. "}},</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="133">
+    <row r="56" spans="1:19" ht="28" customHeight="1">
       <c r="A56" s="8" t="s">
         <v>243</v>
       </c>
@@ -5230,7 +5234,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.069323,47.481309]},"properties":{"id":"BUD5","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Near Boráros tér. Mester-Angyal u.) moderate busy road close to busy roads. many shops. restaurants. building blocks."}},</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="97">
+    <row r="57" spans="1:19" ht="28" customHeight="1">
       <c r="A57" s="8" t="s">
         <v>247</v>
       </c>
@@ -5290,7 +5294,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.069358,47.485891]},"properties":{"id":"BUD6","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1.5,"trafic":1,"info":"(Corvin-negyed) busy intersection with people. traffic. schools and hospital nearby."}},</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="121">
+    <row r="58" spans="1:19" ht="28" customHeight="1">
       <c r="A58" s="8" t="s">
         <v>252</v>
       </c>
@@ -5350,7 +5354,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.066088,47.487658]},"properties":{"id":"BUD7","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1.5,"trafic":1,"info":"(Near Corvin-negyed and Kálvin tér) moderate busy road with many office buildings. building blocks."}},</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="97">
+    <row r="59" spans="1:19" ht="28" customHeight="1">
       <c r="A59" s="8" t="s">
         <v>256</v>
       </c>
@@ -5410,7 +5414,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.06179,47.489297]},"properties":{"id":"BUD8","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Kálvin tér) busy intersection with people. traffic. schools and hospital nearby."}},</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="85">
+    <row r="60" spans="1:19" ht="28" customHeight="1">
       <c r="A60" s="8" t="s">
         <v>260</v>
       </c>
@@ -5470,7 +5474,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.055664,47.510258]},"properties":{"id":"BUD9","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1.5,"trafic":1,"info":"(Nyugati pu) busy intersection with people. traffic. schools and mall nearby."}},</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="97">
+    <row r="61" spans="1:19" ht="28" customHeight="1">
       <c r="A61" s="8" t="s">
         <v>264</v>
       </c>
@@ -5530,7 +5534,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.053931,47.512085]},"properties":{"id":"BUD10","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(near Nyugati pu. Kádár u) moderate busy street with people. traffic. hospital nearby."}},</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="85">
+    <row r="62" spans="1:19" ht="28" customHeight="1">
       <c r="A62" s="8" t="s">
         <v>268</v>
       </c>
@@ -5590,7 +5594,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.037154,47.514736]},"properties":{"id":"BUD11","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Margit krt) busy road with with people. traffic. hospital nearby."}},</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="109">
+    <row r="63" spans="1:19" ht="28" customHeight="1">
       <c r="A63" s="8" t="s">
         <v>272</v>
       </c>
@@ -5650,7 +5654,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.027087,47.507904]},"properties":{"id":"BUD12","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Széna tér) Busy intersection. bus station. with people. traffic. many office buildings. mall."}},</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="73">
+    <row r="64" spans="1:19" ht="28" customHeight="1">
       <c r="A64" s="8" t="s">
         <v>276</v>
       </c>
@@ -5710,7 +5714,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.023974,47.508516]},"properties":{"id":"BUD13","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1.5,"trafic":1,"info":"(near Széna tér) moderate busy street with people. traffic. mall nearby. "}},</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="121">
+    <row r="65" spans="1:19" ht="28" customHeight="1">
       <c r="A65" s="8" t="s">
         <v>280</v>
       </c>
@@ -5770,7 +5774,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.024256,47.501953]},"properties":{"id":"BUD14","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1.5,"trafic":1,"info":"(Déli pu) Busy intersection. bus station. with people. traffic. many office buildings. schools and a big park."}},</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="134" thickBot="1">
+    <row r="66" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A66" s="9" t="s">
         <v>284</v>
       </c>
@@ -5830,7 +5834,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.021809,47.502454]},"properties":{"id":"BUD15","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1.5,"trafic":1,"info":"(near Déli pu. Városmajor u.) moderate busy street with people. traffic. many office buildings. schools and a hospital nearby."}},</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="74" thickBot="1">
+    <row r="67" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A67" s="2" t="s">
         <v>288</v>
       </c>
@@ -5890,7 +5894,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.546835,53.932023]},"properties":{"id":"MSQ1","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":3,"trafic":1,"info":"Busy intersection with heavy truck traffic, pedestrians, bikeroads"}},</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="97">
+    <row r="68" spans="1:19" ht="28" customHeight="1">
       <c r="A68" s="8" t="s">
         <v>224</v>
       </c>
@@ -5950,7 +5954,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.075728,47.467912]},"properties":{"id":"BUD1","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Közvágóhíd megálló) Busy intersection with people, traffic, party places, theatre nearby."}},</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="145">
+    <row r="69" spans="1:19" ht="28" customHeight="1">
       <c r="A69" s="8" t="s">
         <v>231</v>
       </c>
@@ -6010,7 +6014,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.080888,47.466466]},"properties":{"id":"BUD2","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Near Közvágóhíd, Gubacsi út Tesco) moderate busy road close to intersection, people, traffic, party places, and mall close."}},</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="97">
+    <row r="70" spans="1:19" ht="28" customHeight="1">
       <c r="A70" s="8" t="s">
         <v>235</v>
       </c>
@@ -6068,7 +6072,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.067378,47.479634]},"properties":{"id":"BUD3","group":"CAAG","city":"","color":"#3fc9f0","height":2,"trafic":1,"info":"(Boráros tér-fent) Busy intersection, bus station, with people, traffic, many office buildings."}},</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="85">
+    <row r="71" spans="1:19" ht="28" customHeight="1">
       <c r="A71" s="8" t="s">
         <v>239</v>
       </c>
@@ -6128,7 +6132,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.066933,47.479971]},"properties":{"id":"BUD4","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1,"trafic":1,"info":"(Boráros tér -lent) Busy intersection with people, traffic, many office buildings. "}},</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="133">
+    <row r="72" spans="1:19" ht="28" customHeight="1">
       <c r="A72" s="8" t="s">
         <v>243</v>
       </c>
@@ -6188,7 +6192,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.069323,47.481309]},"properties":{"id":"BUD5","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Near Boráros tér, Mester-Angyal u.) moderate busy road close to busy roads, many shops, restaurants, building blocks."}},</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="97">
+    <row r="73" spans="1:19" ht="28" customHeight="1">
       <c r="A73" s="8" t="s">
         <v>247</v>
       </c>
@@ -6248,7 +6252,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.069358,47.485891]},"properties":{"id":"BUD6","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1.5,"trafic":1,"info":"(Corvin-negyed) busy intersection with people, traffic, schools and hospital nearby."}},</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="121">
+    <row r="74" spans="1:19" ht="28" customHeight="1">
       <c r="A74" s="8" t="s">
         <v>252</v>
       </c>
@@ -6308,7 +6312,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.066088,47.487658]},"properties":{"id":"BUD7","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1.5,"trafic":1,"info":"(Near Corvin-negyed and Kálvin tér) moderate busy road with many office buildings, building blocks."}},</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="97">
+    <row r="75" spans="1:19" ht="28" customHeight="1">
       <c r="A75" s="8" t="s">
         <v>256</v>
       </c>
@@ -6368,7 +6372,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.06179,47.489297]},"properties":{"id":"BUD8","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Kálvin tér) busy intersection with people, traffic, schools and hospital nearby."}},</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="85">
+    <row r="76" spans="1:19" ht="28" customHeight="1">
       <c r="A76" s="8" t="s">
         <v>260</v>
       </c>
@@ -6428,7 +6432,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.055664,47.510258]},"properties":{"id":"BUD9","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1.5,"trafic":1,"info":"(Nyugati pu) busy intersection with people, traffic, schools and mall nearby."}},</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="97">
+    <row r="77" spans="1:19" ht="28" customHeight="1">
       <c r="A77" s="8" t="s">
         <v>264</v>
       </c>
@@ -6488,7 +6492,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.053931,47.512085]},"properties":{"id":"BUD10","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(near Nyugati pu, Kádár u) moderate busy street with people, traffic, hospital nearby."}},</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="85">
+    <row r="78" spans="1:19" ht="28" customHeight="1">
       <c r="A78" s="8" t="s">
         <v>268</v>
       </c>
@@ -6548,7 +6552,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.037154,47.514736]},"properties":{"id":"BUD11","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Margit krt) busy road with with people, traffic, hospital nearby,"}},</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="109">
+    <row r="79" spans="1:19" ht="28" customHeight="1">
       <c r="A79" s="8" t="s">
         <v>272</v>
       </c>
@@ -6608,7 +6612,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.027087,47.507904]},"properties":{"id":"BUD12","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Széna tér) Busy intersection, bus station, with people, traffic, many office buildings, mall."}},</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="73">
+    <row r="80" spans="1:19" ht="28" customHeight="1">
       <c r="A80" s="8" t="s">
         <v>276</v>
       </c>
@@ -6668,7 +6672,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.023974,47.508516]},"properties":{"id":"BUD13","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1.5,"trafic":1,"info":"(near Széna tér) moderate busy street with people, traffic, mall nearby. "}},</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="121">
+    <row r="81" spans="1:19" ht="28" customHeight="1">
       <c r="A81" s="8" t="s">
         <v>280</v>
       </c>
@@ -6728,7 +6732,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.024256,47.501953]},"properties":{"id":"BUD14","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1.5,"trafic":1,"info":"(Déli pu) Busy intersection, bus station, with people, traffic, many office buildings, schools and a big park."}},</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="133">
+    <row r="82" spans="1:19" ht="28" customHeight="1">
       <c r="A82" s="11" t="s">
         <v>284</v>
       </c>
@@ -6788,7 +6792,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.021809,47.502454]},"properties":{"id":"BUD15","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1.5,"trafic":1,"info":"(near Déli pu, Városmajor u.) moderate busy street with people, traffic, many office buildings, schools and a hospital nearby."}},</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="97">
+    <row r="83" spans="1:19" ht="28" customHeight="1">
       <c r="A83" s="11" t="s">
         <v>310</v>
       </c>
@@ -6848,7 +6852,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.078942,47.496672]},"properties":{"id":"BUD16","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":0,"info":"(II.János Pál pápa tér), green park surrounded by residential buildings and moderate traffic."}},</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="145">
+    <row r="84" spans="1:19" ht="28" customHeight="1">
       <c r="A84" s="11" t="s">
         <v>314</v>
       </c>
@@ -6908,7 +6912,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.041137,47.540964]},"properties":{"id":"BUD17","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Flórián tér) Busy intersection, bus, tram station, with people, traffic, many resitential buildings, hospital, shopping mall, schools."}},</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="121">
+    <row r="85" spans="1:19" ht="28" customHeight="1">
       <c r="A85" s="11" t="s">
         <v>318</v>
       </c>
@@ -6968,7 +6972,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.038189,47.543455]},"properties":{"id":"BUD18","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(nearFlórián tér, Kórház u.) moderate busy street with many residential building blocks, shops, people, hospital."}},</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="193">
+    <row r="86" spans="1:19" ht="28" customHeight="1">
       <c r="A86" s="11" t="s">
         <v>322</v>
       </c>
@@ -7028,7 +7032,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.088348,47.518866]},"properties":{"id":"BUD19","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Kacsóh Pongrác úti megálló) Busy intersection, entry to highway, bus, tram station, with people, traffic, many resitential buildings,  hospital, close to UNESCO city park and bath."}},</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="145">
+    <row r="87" spans="1:19" ht="28" customHeight="1">
       <c r="A87" s="11" t="s">
         <v>326</v>
       </c>
@@ -7088,7 +7092,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.086176,47.518239]},"properties":{"id":"BUD20","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Near to Kacsóh Pongrác), busy road with public transport, traffic, people,beside the UNESCO city park, residential buildings."}},</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="121">
+    <row r="88" spans="1:19" ht="28" customHeight="1">
       <c r="A88" s="11" t="s">
         <v>330</v>
       </c>
@@ -7148,7 +7152,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.090144,47.560772]},"properties":{"id":"BUD21","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1.5,"trafic":1,"info":"(Újpest-Városközpont) busy intersection with public transport,traffic, people,residential building blocks, shops."}},</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="109">
+    <row r="89" spans="1:19" ht="28" customHeight="1">
       <c r="A89" s="11" t="s">
         <v>334</v>
       </c>
@@ -7208,7 +7212,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.088294,47.561605]},"properties":{"id":"BUD22","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Near Újpest-Városközpont) moderate busy street with a park, residential buildings, mall, shops, traffic."}},</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="97">
+    <row r="90" spans="1:19" ht="28" customHeight="1">
       <c r="A90" s="11" t="s">
         <v>338</v>
       </c>
@@ -7268,7 +7272,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.089486,47.478829]},"properties":{"id":"BUD23","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Nagyvárad tér) busy intersection with traffic, people, school,hospitals, close to green park."}},</v>
       </c>
     </row>
-    <row r="91" spans="1:19">
+    <row r="91" spans="1:19" ht="28" customHeight="1">
       <c r="A91" t="s">
         <v>342</v>
       </c>
@@ -7328,7 +7332,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.094298,47.480592]},"properties":{"id":"BUD24","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(near to Nagyvárad tér), moderate busy street with traffic,people, residential buildings, schools, hospital, close to green park."}},</v>
       </c>
     </row>
-    <row r="92" spans="1:19">
+    <row r="92" spans="1:19" ht="28" customHeight="1">
       <c r="A92" t="s">
         <v>346</v>
       </c>
@@ -7388,7 +7392,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.094559,47.521894]},"properties":{"id":"BUD25","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(near to highway M3 and city park). moderate busy street with people. residential building blocks. traffic."}},</v>
       </c>
     </row>
-    <row r="93" spans="1:19">
+    <row r="93" spans="1:19" ht="28" customHeight="1">
       <c r="A93" t="s">
         <v>350</v>
       </c>
@@ -7448,7 +7452,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.016553,47.466128]},"properties":{"id":"BUD26","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":1,"trafic":1,"info":"(Budaörsi út. near Kelenföld pu) busy road with people. traffic. train and bus station close. residential buildings and offices."}},</v>
       </c>
     </row>
-    <row r="94" spans="1:19">
+    <row r="94" spans="1:19" ht="28" customHeight="1">
       <c r="A94" t="s">
         <v>354</v>
       </c>
@@ -7508,7 +7512,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.019297,47.467142]},"properties":{"id":"BUD27","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(near to Budaörsi út). moderate busy street with people. traffic. residential buildings."}},</v>
       </c>
     </row>
-    <row r="95" spans="1:19">
+    <row r="95" spans="1:19" ht="28" customHeight="1">
       <c r="A95" t="s">
         <v>358</v>
       </c>
@@ -7568,7 +7572,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.136842,47.503904]},"properties":{"id":"BUD28","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(Örs vezér tér) busy intersection with people. traffic. every kind of public transport. shopping mall. close to hospital."}},</v>
       </c>
     </row>
-    <row r="96" spans="1:19">
+    <row r="96" spans="1:19" ht="28" customHeight="1">
       <c r="A96" t="s">
         <v>362</v>
       </c>
@@ -7628,7 +7632,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.133894,47.505597]},"properties":{"id":"BUD29","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":1,"info":"(near to Örs vezér tér).moderate busy street with people. traffic. hospital."}},</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="16" thickBot="1">
+    <row r="97" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A97" t="s">
         <v>366</v>
       </c>
@@ -7688,7 +7692,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[19.100679,47.476853]},"properties":{"id":"BUD30","group":"CAAG","city":"Budapest","color":"#3fc9f0","height":2,"trafic":0/1,"info":"(Népliget). moderate or no traffic. green park. people. close to bus station and busy road."}},</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="86" thickBot="1">
+    <row r="98" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A98" s="13" t="s">
         <v>288</v>
       </c>
@@ -7748,7 +7752,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.546835,53.932023]},"properties":{"id":"MSQ1","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":3,"trafic":1,"info":"Arlouskaya st., busy intersection with heavy truck traffic, pedestrians, bikeroads"}},</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="98" thickBot="1">
+    <row r="99" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A99" s="13" t="s">
         <v>372</v>
       </c>
@@ -7808,7 +7812,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.671079,53.945368]},"properties":{"id":"MSQ2","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":2,"trafic":1,"info":"Uručča, residential area with open access to the heavily loaded outer city ring"}},</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="74" thickBot="1">
+    <row r="100" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A100" s="13" t="s">
         <v>376</v>
       </c>
@@ -7868,7 +7872,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.608928,53.923499]},"properties":{"id":"MSQ3","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":2,"trafic":1,"info":"Independence ave/Kalinina sq., city center, heavy traffic"}},</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="62" thickBot="1">
+    <row r="101" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A101" s="13" t="s">
         <v>380</v>
       </c>
@@ -7928,7 +7932,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.587808,53.920724]},"properties":{"id":"MSQ4","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":3,"trafic":1,"info":"Kolasa st., Technical university campus, heavy traffic"}},</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="74" thickBot="1">
+    <row r="102" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A102" s="13" t="s">
         <v>384</v>
       </c>
@@ -7988,7 +7992,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.580108,53.887069]},"properties":{"id":"MSQ5","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":2,"trafic":1,"info":"Partizansky ave, traffic interchange, heavy traffic, railway nearby"}},</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="50" thickBot="1">
+    <row r="103" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A103" s="13" t="s">
         <v>388</v>
       </c>
@@ -8048,7 +8052,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.609916,53.878242]},"properties":{"id":"MSQ6","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":3,"trafic":1,"info":"Vaneeva st., traffic circle, lots of pedestrians"}},</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="50" thickBot="1">
+    <row r="104" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A104" s="13" t="s">
         <v>392</v>
       </c>
@@ -8108,7 +8112,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.568392,53.875016]},"properties":{"id":"MSQ7","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":3,"trafic":1,"info":"Mayakovskogo st., heavy traffic, pedestrians"}},</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="74" thickBot="1">
+    <row r="105" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A105" s="13" t="s">
         <v>396</v>
       </c>
@@ -8168,7 +8172,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.606739,53.862187]},"properties":{"id":"MSQ8","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":2,"trafic":1,"info":"Plehanova st., main crossroads in large residential district"}},</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="38" thickBot="1">
+    <row r="106" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A106" s="13" t="s">
         <v>400</v>
       </c>
@@ -8228,7 +8232,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.639528,53.892688]},"properties":{"id":"MSQ9","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":3,"trafic":1,"info":"Vaupshasov st., heavy transit traffic"}},</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="86" thickBot="1">
+    <row r="107" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A107" s="13" t="s">
         <v>404</v>
       </c>
@@ -8288,7 +8292,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.655988,53.879158]},"properties":{"id":"MSQ10","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":2,"trafic":1,"info":"Radialnaya, heavy traffic, highly polluted industrial area (tractor works)"}},</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="50" thickBot="1">
+    <row r="108" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A108" s="13" t="s">
         <v>408</v>
       </c>
@@ -8348,7 +8352,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.53292,53.839494]},"properties":{"id":"MSQ11","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":2,"trafic":1,"info":"Kizhevatova st., heavy traffic, city entrance"}},</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="38" thickBot="1">
+    <row r="109" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A109" s="13" t="s">
         <v>412</v>
       </c>
@@ -8408,7 +8412,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.538454,53.895705]},"properties":{"id":"MSQ12","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":2,"trafic":1,"info":"Zetkin st., local traffic interchange"}},</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="50" thickBot="1">
+    <row r="110" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A110" s="13" t="s">
         <v>416</v>
       </c>
@@ -8468,7 +8472,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.497873,53.909921]},"properties":{"id":"MSQ13","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":3,"trafic":1,"info":"Pushkin ave, 2nd city ring, heavy loaded"}},</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="62" thickBot="1">
+    <row r="111" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A111" s="13" t="s">
         <v>420</v>
       </c>
@@ -8528,7 +8532,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.41299,53.916667]},"properties":{"id":"MSQ14","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":2,"trafic":1,"info":"Outer city ring near large residential area"}},</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="98" thickBot="1">
+    <row r="112" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A112" s="13" t="s">
         <v>424</v>
       </c>
@@ -8588,7 +8592,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.523712,53.913358]},"properties":{"id":"MSQ15","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":3,"trafic":1,"info":"Timiryazev st., heavy traffic, next to the reference station of BelHydroMet"}},</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="98" thickBot="1">
+    <row r="113" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A113" s="13" t="s">
         <v>428</v>
       </c>
@@ -8648,7 +8652,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.71229,53.947473]},"properties":{"id":"MSQ16","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":2,"trafic":1,"info":"Uručča, residential area, next to the reference station of BelHydroMet"}},</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="38" thickBot="1">
+    <row r="114" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A114" s="13" t="s">
         <v>432</v>
       </c>
@@ -8708,7 +8712,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.615162,53.913675]},"properties":{"id":"MSQ17","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":2,"trafic":1,"info":"City center, local traffic interchange"}},</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="50" thickBot="1">
+    <row r="115" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A115" s="13" t="s">
         <v>436</v>
       </c>
@@ -8768,7 +8772,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.575205,53.941037]},"properties":{"id":"MSQ18","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":1,"trafic":0,"info":"Mozhaisky st., calm residential area"}},</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="26" thickBot="1">
+    <row r="116" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A116" s="13" t="s">
         <v>440</v>
       </c>
@@ -8828,7 +8832,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.530621,53.969048]},"properties":{"id":"MSQ19","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":3,"trafic":1,"info":"Outer city ring"}},</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="38" thickBot="1">
+    <row r="117" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A117" s="13" t="s">
         <v>432</v>
       </c>
@@ -8888,7 +8892,7 @@
         <v>{"type":"Feature","geometry":{"type":"Point","coordinates":[27.615162,53.913675]},"properties":{"id":"MSQ20","group":"airmq.by","city":"Minsk","color":"#03E2B8","height":2,"trafic":0,"info":"Center of city Botanic garden"}},</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="74" thickBot="1">
+    <row r="118" spans="1:19" ht="28" customHeight="1" thickBot="1">
       <c r="A118" s="13" t="s">
         <v>446</v>
       </c>

</xml_diff>

<commit_message>
added EU stations und dolgoprudny
</commit_message>
<xml_diff>
--- a/doc/Workbook1.xlsx
+++ b/doc/Workbook1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1400" yWindow="5800" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1475,7 +1475,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1488,6 +1488,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1544,7 +1547,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1559,6 +1562,9 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1896,8 +1902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:AZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>